<commit_message>
Adjust pinmap to show prototype state
</commit_message>
<xml_diff>
--- a/docs/SBC_IO.xlsx
+++ b/docs/SBC_IO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwest\dev\HyGenCMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwest\dev\HyGenCMS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="247">
   <si>
     <t>Beaglebone IO</t>
   </si>
@@ -764,6 +764,9 @@
   </si>
   <si>
     <t>OFF switch</t>
+  </si>
+  <si>
+    <t>Generator Amps (prototype)</t>
   </si>
 </sst>
 </file>
@@ -892,7 +895,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -913,6 +916,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1446,8 +1450,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2403,6 +2407,9 @@
       <c r="H41" s="15" t="s">
         <v>65</v>
       </c>
+      <c r="I41" s="18" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">

</xml_diff>